<commit_message>
Update kimai data and hours report generator
</commit_message>
<xml_diff>
--- a/kimai-data/29/pay-period-29.xlsx
+++ b/kimai-data/29/pay-period-29.xlsx
@@ -503,13 +503,13 @@
         <f>F7 + G7</f>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="I7" t="str">
-        <v>Short 80.00 hours</v>
+        <v/>
       </c>
     </row>
     <row r="8">
@@ -607,13 +607,13 @@
         <f>F11 + G11</f>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="I11" t="str">
-        <v>Short 80.00 hours</v>
+        <v/>
       </c>
     </row>
     <row r="12">
@@ -636,10 +636,10 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="I12" t="str">
-        <v>Short 45.00 hours</v>
+        <v>Short 10.00 hours</v>
       </c>
     </row>
     <row r="13">
@@ -1071,6 +1071,12 @@
       <c r="H26">
         <v>80</v>
       </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
@@ -1082,6 +1088,9 @@
       <c r="C27">
         <f>SUM(C28:C33)</f>
       </c>
+      <c r="D27">
+        <v>20</v>
+      </c>
       <c r="E27">
         <v>400</v>
       </c>
@@ -1093,6 +1102,12 @@
       </c>
       <c r="H27">
         <v>80</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -1120,6 +1135,12 @@
       <c r="H28">
         <f>D16</f>
       </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
@@ -1353,6 +1374,84 @@
       </c>
       <c r="H37">
         <f>D25</f>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>Ayooluwa</v>
+      </c>
+      <c r="B38">
+        <f>IF(C38 &gt; 0, TEXT(C38 / E38 * 100, "0.00") &amp; "% Missed", IF(C38 &lt; 0, TEXT(-C38 / E38 * 100, "0.00") &amp; "% Overworked", "No Difference"))</f>
+      </c>
+      <c r="C38">
+        <f>E38 - E16</f>
+      </c>
+      <c r="D38">
+        <f>(G38 * 2) - G16</f>
+      </c>
+      <c r="E38">
+        <f>F38 * 2</f>
+      </c>
+      <c r="F38">
+        <f>G38 + H38</f>
+      </c>
+      <c r="G38">
+        <v>20</v>
+      </c>
+      <c r="H38">
+        <f>D26</f>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>Akshat</v>
+      </c>
+      <c r="B39">
+        <f>IF(C39 &gt; 0, TEXT(C39 / E39 * 100, "0.00") &amp; "% Missed", IF(C39 &lt; 0, TEXT(-C39 / E39 * 100, "0.00") &amp; "% Overworked", "No Difference"))</f>
+      </c>
+      <c r="C39">
+        <f>E39 - E17</f>
+      </c>
+      <c r="D39">
+        <f>(G39 * 2) - G17</f>
+      </c>
+      <c r="E39">
+        <f>F39 * 2</f>
+      </c>
+      <c r="F39">
+        <f>G39 + H39</f>
+      </c>
+      <c r="G39">
+        <v>20</v>
+      </c>
+      <c r="H39">
+        <f>D27</f>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>DJ</v>
+      </c>
+      <c r="B40">
+        <f>IF(C40 &gt; 0, TEXT(C40 / E40 * 100, "0.00") &amp; "% Missed", IF(C40 &lt; 0, TEXT(-C40 / E40 * 100, "0.00") &amp; "% Overworked", "No Difference"))</f>
+      </c>
+      <c r="C40">
+        <f>E40 - E18</f>
+      </c>
+      <c r="D40">
+        <f>(G40 * 2) - G18</f>
+      </c>
+      <c r="E40">
+        <f>F40 * 2</f>
+      </c>
+      <c r="F40">
+        <f>G40 + H40</f>
+      </c>
+      <c r="G40">
+        <v>20</v>
+      </c>
+      <c r="H40">
+        <f>D28</f>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update users configuration and pay period 29 data
</commit_message>
<xml_diff>
--- a/kimai-data/29/pay-period-29.xlsx
+++ b/kimai-data/29/pay-period-29.xlsx
@@ -723,7 +723,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="str">
-        <v>Short 16.82 hours</v>
+        <v>Extra 19.68 hours carry over</v>
       </c>
     </row>
     <row r="16">
@@ -1326,7 +1326,7 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>Forrest Cordova</v>
+        <v>Jamie</v>
       </c>
       <c r="B36">
         <f>IF(C36 &gt; 0, TEXT(C36 / E36 * 100, "0.00") &amp; "% Missed", IF(C36 &lt; 0, TEXT(-C36 / E36 * 100, "0.00") &amp; "% Overworked", "No Difference"))</f>
@@ -1344,7 +1344,7 @@
         <f>G36 + H36</f>
       </c>
       <c r="G36">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="H36">
         <f>D24</f>
@@ -1352,7 +1352,7 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>Jamie</v>
+        <v>Ayooluwa</v>
       </c>
       <c r="B37">
         <f>IF(C37 &gt; 0, TEXT(C37 / E37 * 100, "0.00") &amp; "% Missed", IF(C37 &lt; 0, TEXT(-C37 / E37 * 100, "0.00") &amp; "% Overworked", "No Difference"))</f>
@@ -1378,7 +1378,7 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>Ayooluwa</v>
+        <v>Akshat</v>
       </c>
       <c r="B38">
         <f>IF(C38 &gt; 0, TEXT(C38 / E38 * 100, "0.00") &amp; "% Missed", IF(C38 &lt; 0, TEXT(-C38 / E38 * 100, "0.00") &amp; "% Overworked", "No Difference"))</f>
@@ -1404,7 +1404,7 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>Akshat</v>
+        <v>DJ</v>
       </c>
       <c r="B39">
         <f>IF(C39 &gt; 0, TEXT(C39 / E39 * 100, "0.00") &amp; "% Missed", IF(C39 &lt; 0, TEXT(-C39 / E39 * 100, "0.00") &amp; "% Overworked", "No Difference"))</f>
@@ -1426,32 +1426,6 @@
       </c>
       <c r="H39">
         <f>D27</f>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="str">
-        <v>DJ</v>
-      </c>
-      <c r="B40">
-        <f>IF(C40 &gt; 0, TEXT(C40 / E40 * 100, "0.00") &amp; "% Missed", IF(C40 &lt; 0, TEXT(-C40 / E40 * 100, "0.00") &amp; "% Overworked", "No Difference"))</f>
-      </c>
-      <c r="C40">
-        <f>E40 - E18</f>
-      </c>
-      <c r="D40">
-        <f>(G40 * 2) - G18</f>
-      </c>
-      <c r="E40">
-        <f>F40 * 2</f>
-      </c>
-      <c r="F40">
-        <f>G40 + H40</f>
-      </c>
-      <c r="G40">
-        <v>20</v>
-      </c>
-      <c r="H40">
-        <f>D28</f>
       </c>
     </row>
   </sheetData>

</xml_diff>